<commit_message>
sent contract page is now visable
navigate user to contract sent page

allow user to click on back to procurement dashboard from sent contract page

migrate assm state and add state machine on procurement_suppliers and change state on both model

generate contract number after the user click "send to supplier"
move static text to locale file

Update sort order and display location on procurement dashboard

intergrate gov notify and sent email to chee email address with correct format

corrected header banner for the confract sent page

Changed the method to determine if a contract is closed

Added method to offer to next supplier

Test methods for procurement supplier

Tests for offer to next supplier

renew supplier data and gov notify email will be sent to the supplier email

Code quality refactor

Fix for failing test and update controller
</commit_message>
<xml_diff>
--- a/data/facilities_management/RM3830 Suppliers Details (for Dev & Test).xlsx
+++ b/data/facilities_management/RM3830 Suppliers Details (for Dev & Test).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iceraluk/Projects/crown-marketplace/data/facilities_management/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy.south/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABF52EC-C30C-7247-B5E1-F8D4DFB88AF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5233CE4-122B-B946-92AD-A766406CFC58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RM3830 Suppliers Details" sheetId="7" r:id="rId1"/>
@@ -229,15 +229,6 @@
     <t>rowe-hessel-and-heller@yopmail.com</t>
   </si>
   <si>
-    <t>nader-prosacco-and-gaylord@yopmail.com</t>
-  </si>
-  <si>
-    <t>marvin-kunde-and-cartwright@yopmail.com</t>
-  </si>
-  <si>
-    <t>kunze-langworth-and-parisian@yopmail.com</t>
-  </si>
-  <si>
     <t>bernier-cassin@yopmail.com</t>
   </si>
   <si>
@@ -262,12 +253,6 @@
     <t>treutel-inc@yopmail.com</t>
   </si>
   <si>
-    <t>halvorson-corwin-and-o-connell@yopmail.com</t>
-  </si>
-  <si>
-    <t>shields-ratke-and-parisian@yopmail.com</t>
-  </si>
-  <si>
     <t>o-keefe-mitchell@yopmail.com</t>
   </si>
   <si>
@@ -298,9 +283,6 @@
     <t>abbott-dooley@yopmail.com</t>
   </si>
   <si>
-    <t>gleichner-thiel-and-weissnat@yopmail.com</t>
-  </si>
-  <si>
     <t>hirthe-mills@yopmail.com</t>
   </si>
   <si>
@@ -310,9 +292,6 @@
     <t>dickinson-abbott@yopmail.com</t>
   </si>
   <si>
-    <t>mayert-kohler-and-schowalter@yopmail.com</t>
-  </si>
-  <si>
     <t>dickens-and-sons@yopmail.com</t>
   </si>
   <si>
@@ -358,9 +337,6 @@
     <t>kulas-schultz-and-moore@yopmail.com</t>
   </si>
   <si>
-    <t>lebsack-vandervort-and-veum@yopmail.com</t>
-  </si>
-  <si>
     <t>Lakisha Kovats  </t>
   </si>
   <si>
@@ -1193,6 +1169,30 @@
   </si>
   <si>
     <t>50 Carden Place</t>
+  </si>
+  <si>
+    <t>nader-prosacco-gaylord@yopmail.com</t>
+  </si>
+  <si>
+    <t>marvin-kunde-cartwright@yopmail.com</t>
+  </si>
+  <si>
+    <t>kunze-langworth-parisian@yopmail.com</t>
+  </si>
+  <si>
+    <t>halvorson-corwin-oconnell@yopmail.com</t>
+  </si>
+  <si>
+    <t>shields-ratke-parisian@yopmail.com</t>
+  </si>
+  <si>
+    <t>gleichner-thiel-weissnat@yopmail.com</t>
+  </si>
+  <si>
+    <t>mayert-kohler-schowalter@yopmail.com</t>
+  </si>
+  <si>
+    <t>lebsack-vandervort-veum@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1439,11 +1439,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="21">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1694,51 +1696,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.249977111117893"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2036,6 +1993,13 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2065,13 +2029,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2128,18 +2085,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1541C43-A2EA-DF4D-9DEE-34B2D9C4CC9A}" name="Table1" displayName="Table1" ref="A1:Q48" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1541C43-A2EA-DF4D-9DEE-34B2D9C4CC9A}" name="Table1" displayName="Table1" ref="A1:Q48" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:Q48" xr:uid="{BC26F90D-30B6-BF43-BE43-6F582FC4E0D1}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{3CB64C5D-9500-544A-B0EE-D91E773BFFC7}" name="S/N" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{1DA98F46-B120-E447-8CF2-E3ECC96CFA34}" name="Pseudo names (in Digital Dev)" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{D1080184-CA7C-0749-B3FB-9765C414936F}" name="Lot 1a" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{62A3F65C-45C3-0345-8222-FAB7570B467A}" name="Lot 1b" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{8A42DAD6-FC8A-444A-9555-6C4771C1F427}" name="Lot 1c" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{AA06C492-8108-D04A-AE93-CEF333ECFAFE}" name="Direct Award" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{CB49B323-9962-5541-A35F-5A9328698AD2}" name="SME?" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{C53EA3CA-90F6-EF4B-8C73-27AC8816B49D}" name="Emptoris (esourcing) Contact Name" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{F94F77D5-C9AD-7040-AE57-BA6CF52AF9AE}" name="Emptoris (esourcing) Contact Email" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{3CB64C5D-9500-544A-B0EE-D91E773BFFC7}" name="S/N" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{1DA98F46-B120-E447-8CF2-E3ECC96CFA34}" name="Pseudo names (in Digital Dev)" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{D1080184-CA7C-0749-B3FB-9765C414936F}" name="Lot 1a" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{62A3F65C-45C3-0345-8222-FAB7570B467A}" name="Lot 1b" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{8A42DAD6-FC8A-444A-9555-6C4771C1F427}" name="Lot 1c" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{AA06C492-8108-D04A-AE93-CEF333ECFAFE}" name="Direct Award" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{CB49B323-9962-5541-A35F-5A9328698AD2}" name="SME?" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{C53EA3CA-90F6-EF4B-8C73-27AC8816B49D}" name="Emptoris (esourcing) Contact Name" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{F94F77D5-C9AD-7040-AE57-BA6CF52AF9AE}" name="Emptoris (esourcing) Contact Email"/>
     <tableColumn id="3" xr3:uid="{0D98E1E8-9383-BA44-A6B2-D7A907A376A9}" name="Emptoris (esourcing) Contact Number" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{983F1DA7-6A9D-6641-AA15-6641DAB844B4}" name="DUNS number" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{DE3C212D-00A5-8149-99D2-99DCDCC59A1B}" name="Registration number" dataDxfId="5"/>
@@ -2452,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EF542E-3315-DB42-B6D5-B548DE01FA5C}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="213" zoomScaleNormal="213" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2481,16 +2438,16 @@
         <v>13</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>64</v>
@@ -2511,19 +2468,19 @@
         <v>1</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2535,10 +2492,10 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>61</v>
@@ -2547,13 +2504,13 @@
         <v>61</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="I2" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>65</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="K2" s="10">
         <v>764282745</v>
@@ -2562,19 +2519,19 @@
         <v>2564794</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2585,10 +2542,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="16" t="s">
@@ -2598,13 +2555,13 @@
         <v>61</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I3" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>66</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="K3" s="10">
         <v>236500950</v>
@@ -2613,19 +2570,19 @@
         <v>2</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2636,10 +2593,10 @@
         <v>16</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="16" t="s">
@@ -2649,13 +2606,13 @@
         <v>61</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="I4" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>67</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="K4" s="10">
         <v>490446085</v>
@@ -2664,19 +2621,19 @@
         <v>3075427</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2688,10 +2645,10 @@
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>61</v>
@@ -2700,13 +2657,13 @@
         <v>61</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>68</v>
+        <v>107</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>382</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="K5" s="10">
         <v>222252038</v>
@@ -2715,19 +2672,19 @@
         <v>4243192</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2738,10 +2695,10 @@
         <v>18</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="16" t="s">
@@ -2751,13 +2708,13 @@
         <v>61</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>69</v>
+        <v>108</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>383</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K6" s="10">
         <v>289857096</v>
@@ -2766,19 +2723,19 @@
         <v>1799580</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2789,7 +2746,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -2800,13 +2757,13 @@
         <v>62</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>70</v>
+        <v>109</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>384</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="K7" s="10">
         <v>896161635</v>
@@ -2815,19 +2772,19 @@
         <v>3313671</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2839,10 +2796,10 @@
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>61</v>
@@ -2851,26 +2808,26 @@
         <v>61</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>71</v>
+        <v>110</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="K8" s="10">
         <v>864282731</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="11" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2882,10 +2839,10 @@
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>61</v>
@@ -2894,13 +2851,13 @@
         <v>61</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>72</v>
+        <v>111</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>69</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="K9" s="10">
         <v>210330247</v>
@@ -2909,19 +2866,19 @@
         <v>806888</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2932,10 +2889,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="16" t="s">
@@ -2945,13 +2902,13 @@
         <v>62</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>73</v>
+        <v>112</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>70</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="K10" s="10">
         <v>211561968</v>
@@ -2960,19 +2917,19 @@
         <v>3</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2983,7 +2940,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
@@ -2994,13 +2951,13 @@
         <v>61</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>74</v>
+        <v>113</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>71</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="K11" s="10">
         <v>217198175</v>
@@ -3009,19 +2966,19 @@
         <v>665702</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3033,10 +2990,10 @@
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>61</v>
@@ -3045,13 +3002,13 @@
         <v>61</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>75</v>
+        <v>114</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>72</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="K12" s="10">
         <v>225072453</v>
@@ -3060,19 +3017,19 @@
         <v>598379</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3083,10 +3040,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="16" t="s">
@@ -3096,13 +3053,13 @@
         <v>61</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>76</v>
+        <v>115</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="K13" s="10">
         <v>392303327</v>
@@ -3111,19 +3068,19 @@
         <v>2114954</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3134,7 +3091,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -3145,13 +3102,13 @@
         <v>61</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>77</v>
+        <v>116</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="K14" s="10">
         <v>222135670</v>
@@ -3160,19 +3117,19 @@
         <v>4</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3184,10 +3141,10 @@
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>61</v>
@@ -3196,13 +3153,13 @@
         <v>61</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>78</v>
+        <v>117</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>75</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="K15" s="10">
         <v>385644406</v>
@@ -3211,19 +3168,19 @@
         <v>3333860</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3234,10 +3191,10 @@
         <v>28</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="16" t="s">
@@ -3247,13 +3204,13 @@
         <v>61</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>79</v>
+        <v>118</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>385</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="K16" s="10">
         <v>211457434</v>
@@ -3262,16 +3219,16 @@
         <v>5</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3282,7 +3239,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -3293,13 +3250,13 @@
         <v>61</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>80</v>
+        <v>119</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>386</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="K17" s="10">
         <v>736978623</v>
@@ -3308,19 +3265,19 @@
         <v>4956673</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3331,10 +3288,10 @@
         <v>30</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="16" t="s">
@@ -3344,13 +3301,13 @@
         <v>61</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>81</v>
+        <v>120</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="K18" s="10">
         <v>719264843</v>
@@ -3359,16 +3316,16 @@
         <v>5307588</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3380,10 +3337,10 @@
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>61</v>
@@ -3392,13 +3349,13 @@
         <v>61</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>82</v>
+        <v>121</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="K19" s="10">
         <v>525682399</v>
@@ -3407,19 +3364,19 @@
         <v>3253304</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3439,13 +3396,13 @@
         <v>61</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>83</v>
+        <v>122</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="K20" s="10">
         <v>293685244</v>
@@ -3454,19 +3411,19 @@
         <v>890885</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3477,10 +3434,10 @@
         <v>33</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="16" t="s">
@@ -3490,13 +3447,13 @@
         <v>61</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>84</v>
+        <v>123</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>79</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="K21" s="10">
         <v>228653481</v>
@@ -3505,19 +3462,19 @@
         <v>1659837</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3530,7 +3487,7 @@
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>61</v>
@@ -3539,13 +3496,13 @@
         <v>61</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>85</v>
+        <v>124</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>80</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="K22" s="10">
         <v>217343180</v>
@@ -3554,16 +3511,16 @@
         <v>6</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3574,7 +3531,7 @@
         <v>35</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -3585,13 +3542,13 @@
         <v>62</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>86</v>
+        <v>125</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="K23" s="10">
         <v>236681271</v>
@@ -3600,19 +3557,19 @@
         <v>3663128</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3624,10 +3581,10 @@
       </c>
       <c r="C24" s="22"/>
       <c r="D24" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>61</v>
@@ -3636,13 +3593,13 @@
         <v>61</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>87</v>
+        <v>126</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="K24" s="10">
         <v>769605726</v>
@@ -3651,19 +3608,19 @@
         <v>2624887</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3675,10 +3632,10 @@
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>61</v>
@@ -3687,13 +3644,13 @@
         <v>61</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>88</v>
+        <v>127</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>83</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="K25" s="10">
         <v>424622228</v>
@@ -3702,16 +3659,16 @@
         <v>4449811</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3722,7 +3679,7 @@
         <v>38</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
@@ -3733,13 +3690,13 @@
         <v>62</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>89</v>
+        <v>128</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="K26" s="10">
         <v>213169964</v>
@@ -3748,19 +3705,19 @@
         <v>1021959</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3772,10 +3729,10 @@
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>61</v>
@@ -3784,13 +3741,13 @@
         <v>61</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>90</v>
+        <v>129</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="K27" s="10">
         <v>505712836</v>
@@ -3799,19 +3756,19 @@
         <v>2519234</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3823,10 +3780,10 @@
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>61</v>
@@ -3835,13 +3792,13 @@
         <v>61</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>91</v>
+        <v>130</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="K28" s="10">
         <v>231384041</v>
@@ -3850,19 +3807,19 @@
         <v>2938041</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3873,7 +3830,7 @@
         <v>41</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -3884,13 +3841,13 @@
         <v>61</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>92</v>
+        <v>131</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="K29" s="10">
         <v>217147297</v>
@@ -3899,19 +3856,19 @@
         <v>906936</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3922,10 +3879,10 @@
         <v>42</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="16" t="s">
@@ -3935,13 +3892,13 @@
         <v>61</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>93</v>
+        <v>132</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K30" s="10">
         <v>671506637</v>
@@ -3950,19 +3907,19 @@
         <v>6009150</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3973,10 +3930,10 @@
         <v>43</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E31" s="22"/>
       <c r="F31" s="16" t="s">
@@ -3986,13 +3943,13 @@
         <v>61</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>94</v>
+        <v>133</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>88</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="K31" s="10">
         <v>346669703</v>
@@ -4001,16 +3958,16 @@
         <v>5472032</v>
       </c>
       <c r="M31" s="11" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4022,10 +3979,10 @@
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>61</v>
@@ -4034,13 +3991,13 @@
         <v>61</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="I32" s="18" t="s">
-        <v>95</v>
+        <v>134</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>388</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K32" s="10">
         <v>211306976</v>
@@ -4049,16 +4006,16 @@
         <v>6647559</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4070,10 +4027,10 @@
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>61</v>
@@ -4082,13 +4039,13 @@
         <v>61</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>96</v>
+        <v>135</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="K33" s="10">
         <v>230367153</v>
@@ -4097,19 +4054,19 @@
         <v>3056469</v>
       </c>
       <c r="M33" s="11" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4120,10 +4077,10 @@
         <v>46</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="16" t="s">
@@ -4133,13 +4090,13 @@
         <v>62</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="I34" s="18" t="s">
-        <v>97</v>
+        <v>136</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>90</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="K34" s="10">
         <v>220175238</v>
@@ -4148,19 +4105,19 @@
         <v>9070750</v>
       </c>
       <c r="M34" s="11" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4173,7 +4130,7 @@
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>61</v>
@@ -4182,13 +4139,13 @@
         <v>62</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>98</v>
+        <v>137</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="J35" s="18" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="K35" s="10">
         <v>234565877</v>
@@ -4197,19 +4154,19 @@
         <v>2792044</v>
       </c>
       <c r="M35" s="11" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4220,10 +4177,10 @@
         <v>48</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="16" t="s">
@@ -4233,13 +4190,13 @@
         <v>61</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="I36" s="18" t="s">
-        <v>99</v>
+        <v>138</v>
+      </c>
+      <c r="I36" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="K36" s="10">
         <v>235690935</v>
@@ -4248,19 +4205,19 @@
         <v>7</v>
       </c>
       <c r="M36" s="11" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4271,7 +4228,7 @@
         <v>49</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -4282,13 +4239,13 @@
         <v>62</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>100</v>
+        <v>139</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="K37" s="10">
         <v>520036930</v>
@@ -4297,19 +4254,19 @@
         <v>3370704</v>
       </c>
       <c r="M37" s="11" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4321,10 +4278,10 @@
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>61</v>
@@ -4333,13 +4290,13 @@
         <v>61</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="I38" s="18" t="s">
-        <v>101</v>
+        <v>140</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="K38" s="10">
         <v>218275036</v>
@@ -4348,19 +4305,19 @@
         <v>7977934</v>
       </c>
       <c r="M38" s="11" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4371,7 +4328,7 @@
         <v>51</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -4382,13 +4339,13 @@
         <v>62</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="I39" s="18" t="s">
-        <v>102</v>
+        <v>141</v>
+      </c>
+      <c r="I39" s="23" t="s">
+        <v>95</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="K39" s="10">
         <v>232920962</v>
@@ -4397,19 +4354,19 @@
         <v>4441132</v>
       </c>
       <c r="M39" s="11" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4420,7 +4377,7 @@
         <v>52</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -4431,13 +4388,13 @@
         <v>61</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="I40" s="18" t="s">
-        <v>103</v>
+        <v>142</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>96</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="K40" s="10">
         <v>214057796</v>
@@ -4446,19 +4403,19 @@
         <v>8</v>
       </c>
       <c r="M40" s="11" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4470,10 +4427,10 @@
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>62</v>
@@ -4482,13 +4439,13 @@
         <v>61</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="I41" s="18" t="s">
-        <v>104</v>
+        <v>143</v>
+      </c>
+      <c r="I41" s="23" t="s">
+        <v>97</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="K41" s="10">
         <v>216308056</v>
@@ -4497,19 +4454,19 @@
         <v>242246</v>
       </c>
       <c r="M41" s="11" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4521,10 +4478,10 @@
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>61</v>
@@ -4533,13 +4490,13 @@
         <v>61</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="I42" s="18" t="s">
-        <v>105</v>
+        <v>144</v>
+      </c>
+      <c r="I42" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="J42" s="18" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="K42" s="10">
         <v>210123801</v>
@@ -4548,19 +4505,19 @@
         <v>6355228</v>
       </c>
       <c r="M42" s="11" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4571,10 +4528,10 @@
         <v>55</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="16" t="s">
@@ -4584,13 +4541,13 @@
         <v>61</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="I43" s="18" t="s">
-        <v>106</v>
+        <v>145</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="J43" s="18" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="K43" s="10">
         <v>212450233</v>
@@ -4599,19 +4556,19 @@
         <v>690190</v>
       </c>
       <c r="M43" s="11" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4623,10 +4580,10 @@
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>61</v>
@@ -4635,13 +4592,13 @@
         <v>61</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="I44" s="18" t="s">
-        <v>107</v>
+        <v>146</v>
+      </c>
+      <c r="I44" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="K44" s="10">
         <v>217253889</v>
@@ -4650,19 +4607,19 @@
         <v>191408</v>
       </c>
       <c r="M44" s="11" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4673,7 +4630,7 @@
         <v>57</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
@@ -4684,13 +4641,13 @@
         <v>62</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="I45" s="18" t="s">
-        <v>108</v>
+        <v>147</v>
+      </c>
+      <c r="I45" s="23" t="s">
+        <v>101</v>
       </c>
       <c r="J45" s="18" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="K45" s="10">
         <v>210978877</v>
@@ -4699,19 +4656,19 @@
         <v>6421189</v>
       </c>
       <c r="M45" s="11" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4723,10 +4680,10 @@
       </c>
       <c r="C46" s="22"/>
       <c r="D46" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>61</v>
@@ -4735,13 +4692,13 @@
         <v>61</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="I46" s="18" t="s">
-        <v>109</v>
+        <v>148</v>
+      </c>
+      <c r="I46" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="K46" s="10">
         <v>210354460</v>
@@ -4750,19 +4707,19 @@
         <v>842846</v>
       </c>
       <c r="M46" s="11" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4773,7 +4730,7 @@
         <v>59</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
@@ -4784,13 +4741,13 @@
         <v>62</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="I47" s="18" t="s">
-        <v>110</v>
+        <v>149</v>
+      </c>
+      <c r="I47" s="23" t="s">
+        <v>103</v>
       </c>
       <c r="J47" s="18" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="K47" s="10">
         <v>846921898</v>
@@ -4799,16 +4756,16 @@
         <v>9</v>
       </c>
       <c r="M47" s="11" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4819,10 +4776,10 @@
         <v>60</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="17" t="s">
@@ -4832,13 +4789,13 @@
         <v>61</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="I48" s="18" t="s">
-        <v>111</v>
+        <v>150</v>
+      </c>
+      <c r="I48" s="23" t="s">
+        <v>389</v>
       </c>
       <c r="J48" s="18" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="K48" s="14">
         <v>500063557</v>
@@ -4847,28 +4804,25 @@
         <v>2295904</v>
       </c>
       <c r="M48" s="15" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="mann@yopmail.com" xr:uid="{B1FBFBC1-9792-104B-B9DA-E169C34BD73C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated json with correct supplier emails
Change to use corrected emails

Removed unesecery page titles from router

Update supplier email

Updated the dashboard to show the correct details

Sorted the results

Added routes for the supplier contracts pages

Fix code quality issues

Sort the ordering of the contracts
</commit_message>
<xml_diff>
--- a/data/facilities_management/RM3830 Suppliers Details (for Dev & Test).xlsx
+++ b/data/facilities_management/RM3830 Suppliers Details (for Dev & Test).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy.south/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5233CE4-122B-B946-92AD-A766406CFC58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E377402-55A7-CF41-8AF5-16BC60EF141C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RM3830 Suppliers Details" sheetId="7" r:id="rId1"/>
@@ -328,9 +328,6 @@
     <t>krajcik-gibson@yopmail.com</t>
   </si>
   <si>
-    <t>ullrich-ratke-and-botsford@yopmail.com</t>
-  </si>
-  <si>
     <t>smitham-brown@yopmail.com</t>
   </si>
   <si>
@@ -1193,13 +1190,16 @@
   </si>
   <si>
     <t>lebsack-vandervort-veum@yopmail.com</t>
+  </si>
+  <si>
+    <t>ullrich-ratke-botsford@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1240,6 +1240,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1370,10 +1377,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1441,8 +1449,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
@@ -1993,13 +2003,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2029,6 +2032,13 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2085,7 +2095,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1541C43-A2EA-DF4D-9DEE-34B2D9C4CC9A}" name="Table1" displayName="Table1" ref="A1:Q48" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1541C43-A2EA-DF4D-9DEE-34B2D9C4CC9A}" name="Table1" displayName="Table1" ref="A1:Q48" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:Q48" xr:uid="{BC26F90D-30B6-BF43-BE43-6F582FC4E0D1}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{3CB64C5D-9500-544A-B0EE-D91E773BFFC7}" name="S/N" dataDxfId="15"/>
@@ -2409,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EF542E-3315-DB42-B6D5-B548DE01FA5C}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="C23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2438,16 +2448,16 @@
         <v>13</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="E1" s="21" t="s">
-        <v>201</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>64</v>
@@ -2468,19 +2478,19 @@
         <v>1</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2492,10 +2502,10 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>61</v>
@@ -2504,13 +2514,13 @@
         <v>61</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>65</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K2" s="10">
         <v>764282745</v>
@@ -2519,19 +2529,19 @@
         <v>2564794</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2542,10 +2552,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="16" t="s">
@@ -2555,13 +2565,13 @@
         <v>61</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I3" s="23" t="s">
         <v>66</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K3" s="10">
         <v>236500950</v>
@@ -2570,19 +2580,19 @@
         <v>2</v>
       </c>
       <c r="M3" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2593,10 +2603,10 @@
         <v>16</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="16" t="s">
@@ -2606,13 +2616,13 @@
         <v>61</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I4" s="23" t="s">
         <v>67</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K4" s="10">
         <v>490446085</v>
@@ -2621,19 +2631,19 @@
         <v>3075427</v>
       </c>
       <c r="M4" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2645,10 +2655,10 @@
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>61</v>
@@ -2657,13 +2667,13 @@
         <v>61</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K5" s="10">
         <v>222252038</v>
@@ -2672,19 +2682,19 @@
         <v>4243192</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N5" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2695,10 +2705,10 @@
         <v>18</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="16" t="s">
@@ -2708,13 +2718,13 @@
         <v>61</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K6" s="10">
         <v>289857096</v>
@@ -2723,19 +2733,19 @@
         <v>1799580</v>
       </c>
       <c r="M6" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q6" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2746,7 +2756,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -2757,13 +2767,13 @@
         <v>62</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K7" s="10">
         <v>896161635</v>
@@ -2772,19 +2782,19 @@
         <v>3313671</v>
       </c>
       <c r="M7" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2796,10 +2806,10 @@
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>61</v>
@@ -2808,26 +2818,26 @@
         <v>61</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>68</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K8" s="10">
         <v>864282731</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2839,10 +2849,10 @@
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>61</v>
@@ -2851,13 +2861,13 @@
         <v>61</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I9" s="23" t="s">
         <v>69</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K9" s="10">
         <v>210330247</v>
@@ -2866,19 +2876,19 @@
         <v>806888</v>
       </c>
       <c r="M9" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2889,10 +2899,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="16" t="s">
@@ -2902,13 +2912,13 @@
         <v>62</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I10" s="23" t="s">
         <v>70</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K10" s="10">
         <v>211561968</v>
@@ -2917,19 +2927,19 @@
         <v>3</v>
       </c>
       <c r="M10" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="O10" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2940,7 +2950,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
@@ -2951,13 +2961,13 @@
         <v>61</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I11" s="23" t="s">
         <v>71</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K11" s="10">
         <v>217198175</v>
@@ -2966,19 +2976,19 @@
         <v>665702</v>
       </c>
       <c r="M11" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="O11" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="P11" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="Q11" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2990,10 +3000,10 @@
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>61</v>
@@ -3002,13 +3012,13 @@
         <v>61</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>72</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K12" s="10">
         <v>225072453</v>
@@ -3017,19 +3027,19 @@
         <v>598379</v>
       </c>
       <c r="M12" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="O12" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="Q12" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3040,10 +3050,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="16" t="s">
@@ -3053,13 +3063,13 @@
         <v>61</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>73</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K13" s="10">
         <v>392303327</v>
@@ -3068,19 +3078,19 @@
         <v>2114954</v>
       </c>
       <c r="M13" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="Q13" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3091,7 +3101,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -3102,13 +3112,13 @@
         <v>61</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I14" s="23" t="s">
         <v>74</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K14" s="10">
         <v>222135670</v>
@@ -3117,19 +3127,19 @@
         <v>4</v>
       </c>
       <c r="M14" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="N14" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="O14" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3141,10 +3151,10 @@
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>61</v>
@@ -3153,13 +3163,13 @@
         <v>61</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I15" s="23" t="s">
         <v>75</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K15" s="10">
         <v>385644406</v>
@@ -3168,19 +3178,19 @@
         <v>3333860</v>
       </c>
       <c r="M15" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="O15" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="Q15" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3191,10 +3201,10 @@
         <v>28</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="16" t="s">
@@ -3204,13 +3214,13 @@
         <v>61</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K16" s="10">
         <v>211457434</v>
@@ -3219,16 +3229,16 @@
         <v>5</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3239,7 +3249,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -3250,13 +3260,13 @@
         <v>61</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K17" s="10">
         <v>736978623</v>
@@ -3265,19 +3275,19 @@
         <v>4956673</v>
       </c>
       <c r="M17" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>272</v>
-      </c>
       <c r="O17" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3288,10 +3298,10 @@
         <v>30</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="16" t="s">
@@ -3301,13 +3311,13 @@
         <v>61</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I18" s="23" t="s">
         <v>76</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K18" s="10">
         <v>719264843</v>
@@ -3316,16 +3326,16 @@
         <v>5307588</v>
       </c>
       <c r="M18" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q18" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3337,10 +3347,10 @@
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>61</v>
@@ -3349,13 +3359,13 @@
         <v>61</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I19" s="23" t="s">
         <v>77</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K19" s="10">
         <v>525682399</v>
@@ -3364,19 +3374,19 @@
         <v>3253304</v>
       </c>
       <c r="M19" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="O19" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3396,13 +3406,13 @@
         <v>61</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>78</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K20" s="10">
         <v>293685244</v>
@@ -3411,19 +3421,19 @@
         <v>890885</v>
       </c>
       <c r="M20" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="O20" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3434,10 +3444,10 @@
         <v>33</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="16" t="s">
@@ -3447,13 +3457,13 @@
         <v>61</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I21" s="23" t="s">
         <v>79</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K21" s="10">
         <v>228653481</v>
@@ -3462,19 +3472,19 @@
         <v>1659837</v>
       </c>
       <c r="M21" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="O21" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3487,7 +3497,7 @@
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>61</v>
@@ -3496,13 +3506,13 @@
         <v>61</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I22" s="23" t="s">
         <v>80</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K22" s="10">
         <v>217343180</v>
@@ -3511,16 +3521,16 @@
         <v>6</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3531,7 +3541,7 @@
         <v>35</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -3542,13 +3552,13 @@
         <v>62</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I23" s="23" t="s">
         <v>81</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K23" s="10">
         <v>236681271</v>
@@ -3557,19 +3567,19 @@
         <v>3663128</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N23" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="O23" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="Q23" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3581,10 +3591,10 @@
       </c>
       <c r="C24" s="22"/>
       <c r="D24" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>61</v>
@@ -3593,13 +3603,13 @@
         <v>61</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I24" s="23" t="s">
         <v>82</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K24" s="10">
         <v>769605726</v>
@@ -3608,19 +3618,19 @@
         <v>2624887</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N24" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="O24" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="P24" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="Q24" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3632,10 +3642,10 @@
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>61</v>
@@ -3644,13 +3654,13 @@
         <v>61</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I25" s="23" t="s">
         <v>83</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K25" s="10">
         <v>424622228</v>
@@ -3659,16 +3669,16 @@
         <v>4449811</v>
       </c>
       <c r="M25" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q25" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3679,7 +3689,7 @@
         <v>38</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
@@ -3690,13 +3700,13 @@
         <v>62</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I26" s="23" t="s">
         <v>84</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K26" s="10">
         <v>213169964</v>
@@ -3705,19 +3715,19 @@
         <v>1021959</v>
       </c>
       <c r="M26" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="N26" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="N26" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="O26" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3729,10 +3739,10 @@
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>61</v>
@@ -3741,13 +3751,13 @@
         <v>61</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I27" s="23" t="s">
         <v>85</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K27" s="10">
         <v>505712836</v>
@@ -3756,19 +3766,19 @@
         <v>2519234</v>
       </c>
       <c r="M27" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="N27" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="N27" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="O27" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3780,10 +3790,10 @@
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>61</v>
@@ -3792,13 +3802,13 @@
         <v>61</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K28" s="10">
         <v>231384041</v>
@@ -3807,19 +3817,19 @@
         <v>2938041</v>
       </c>
       <c r="M28" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="N28" s="2" t="s">
-        <v>308</v>
-      </c>
       <c r="O28" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P28" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="P28" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="Q28" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3830,7 +3840,7 @@
         <v>41</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -3841,13 +3851,13 @@
         <v>61</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I29" s="23" t="s">
         <v>86</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K29" s="10">
         <v>217147297</v>
@@ -3856,19 +3866,19 @@
         <v>906936</v>
       </c>
       <c r="M29" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="N29" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="N29" s="2" t="s">
-        <v>308</v>
-      </c>
       <c r="O29" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P29" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="P29" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="Q29" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3879,10 +3889,10 @@
         <v>42</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="16" t="s">
@@ -3892,13 +3902,13 @@
         <v>61</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I30" s="23" t="s">
         <v>87</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K30" s="10">
         <v>671506637</v>
@@ -3907,19 +3917,19 @@
         <v>6009150</v>
       </c>
       <c r="M30" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="N30" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="N30" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="O30" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3930,10 +3940,10 @@
         <v>43</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E31" s="22"/>
       <c r="F31" s="16" t="s">
@@ -3943,13 +3953,13 @@
         <v>61</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I31" s="23" t="s">
         <v>88</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K31" s="10">
         <v>346669703</v>
@@ -3958,16 +3968,16 @@
         <v>5472032</v>
       </c>
       <c r="M31" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3979,10 +3989,10 @@
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>61</v>
@@ -3991,13 +4001,13 @@
         <v>61</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K32" s="10">
         <v>211306976</v>
@@ -4006,16 +4016,16 @@
         <v>6647559</v>
       </c>
       <c r="M32" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="N32" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="N32" s="2" t="s">
-        <v>320</v>
-      </c>
       <c r="O32" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4027,10 +4037,10 @@
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>61</v>
@@ -4039,13 +4049,13 @@
         <v>61</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I33" s="23" t="s">
         <v>89</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K33" s="10">
         <v>230367153</v>
@@ -4054,19 +4064,19 @@
         <v>3056469</v>
       </c>
       <c r="M33" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="N33" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="N33" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="O33" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4077,10 +4087,10 @@
         <v>46</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="16" t="s">
@@ -4090,13 +4100,13 @@
         <v>62</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I34" s="23" t="s">
         <v>90</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K34" s="10">
         <v>220175238</v>
@@ -4105,19 +4115,19 @@
         <v>9070750</v>
       </c>
       <c r="M34" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="N34" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="P34" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q34" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4130,7 +4140,7 @@
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>61</v>
@@ -4139,13 +4149,13 @@
         <v>62</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I35" s="23" t="s">
         <v>91</v>
       </c>
       <c r="J35" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K35" s="10">
         <v>234565877</v>
@@ -4154,19 +4164,19 @@
         <v>2792044</v>
       </c>
       <c r="M35" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="N35" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="N35" s="2" t="s">
+      <c r="O35" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="P35" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="O35" s="2" t="s">
+      <c r="Q35" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4177,10 +4187,10 @@
         <v>48</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="16" t="s">
@@ -4190,13 +4200,13 @@
         <v>61</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I36" s="23" t="s">
         <v>92</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K36" s="10">
         <v>235690935</v>
@@ -4205,19 +4215,19 @@
         <v>7</v>
       </c>
       <c r="M36" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="N36" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="N36" s="2" t="s">
+      <c r="O36" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="O36" s="2" t="s">
+      <c r="P36" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="P36" s="2" t="s">
+      <c r="Q36" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4228,7 +4238,7 @@
         <v>49</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -4239,13 +4249,13 @@
         <v>62</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I37" s="23" t="s">
         <v>93</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K37" s="10">
         <v>520036930</v>
@@ -4254,19 +4264,19 @@
         <v>3370704</v>
       </c>
       <c r="M37" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="O37" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="N37" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="O37" s="2" t="s">
+      <c r="P37" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q37" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4278,10 +4288,10 @@
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>61</v>
@@ -4290,13 +4300,13 @@
         <v>61</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I38" s="23" t="s">
         <v>94</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K38" s="10">
         <v>218275036</v>
@@ -4305,19 +4315,19 @@
         <v>7977934</v>
       </c>
       <c r="M38" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="N38" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="O38" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q38" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4328,7 +4338,7 @@
         <v>51</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -4339,13 +4349,13 @@
         <v>62</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I39" s="23" t="s">
         <v>95</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K39" s="10">
         <v>232920962</v>
@@ -4354,19 +4364,19 @@
         <v>4441132</v>
       </c>
       <c r="M39" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="O39" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="P39" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q39" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="Q39" s="2" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4377,7 +4387,7 @@
         <v>52</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -4388,13 +4398,13 @@
         <v>61</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I40" s="23" t="s">
         <v>96</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K40" s="10">
         <v>214057796</v>
@@ -4403,19 +4413,19 @@
         <v>8</v>
       </c>
       <c r="M40" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="N40" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="N40" s="2" t="s">
-        <v>355</v>
-      </c>
       <c r="O40" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4427,10 +4437,10 @@
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>62</v>
@@ -4439,13 +4449,13 @@
         <v>61</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I41" s="23" t="s">
         <v>97</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K41" s="10">
         <v>216308056</v>
@@ -4454,19 +4464,19 @@
         <v>242246</v>
       </c>
       <c r="M41" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="N41" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="N41" s="2" t="s">
-        <v>359</v>
-      </c>
       <c r="O41" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q41" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4478,10 +4488,10 @@
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>61</v>
@@ -4490,13 +4500,13 @@
         <v>61</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I42" s="23" t="s">
         <v>98</v>
       </c>
       <c r="J42" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K42" s="10">
         <v>210123801</v>
@@ -4505,19 +4515,19 @@
         <v>6355228</v>
       </c>
       <c r="M42" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="N42" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="N42" s="2" t="s">
-        <v>355</v>
-      </c>
       <c r="O42" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4528,10 +4538,10 @@
         <v>55</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="16" t="s">
@@ -4541,13 +4551,13 @@
         <v>61</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I43" s="23" t="s">
         <v>99</v>
       </c>
       <c r="J43" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K43" s="10">
         <v>212450233</v>
@@ -4556,19 +4566,19 @@
         <v>690190</v>
       </c>
       <c r="M43" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="N43" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="N43" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="O43" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4580,10 +4590,10 @@
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>61</v>
@@ -4592,13 +4602,13 @@
         <v>61</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I44" s="23" t="s">
         <v>100</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K44" s="10">
         <v>217253889</v>
@@ -4607,19 +4617,19 @@
         <v>191408</v>
       </c>
       <c r="M44" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="N44" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N44" s="2" t="s">
-        <v>367</v>
-      </c>
       <c r="O44" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4630,7 +4640,7 @@
         <v>57</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
@@ -4641,13 +4651,13 @@
         <v>62</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>101</v>
+        <v>146</v>
+      </c>
+      <c r="I45" s="25" t="s">
+        <v>389</v>
       </c>
       <c r="J45" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K45" s="10">
         <v>210978877</v>
@@ -4656,19 +4666,19 @@
         <v>6421189</v>
       </c>
       <c r="M45" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="N45" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="N45" s="2" t="s">
-        <v>372</v>
-      </c>
       <c r="O45" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4680,10 +4690,10 @@
       </c>
       <c r="C46" s="22"/>
       <c r="D46" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>61</v>
@@ -4692,13 +4702,13 @@
         <v>61</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I46" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K46" s="10">
         <v>210354460</v>
@@ -4707,19 +4717,19 @@
         <v>842846</v>
       </c>
       <c r="M46" s="11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4730,7 +4740,7 @@
         <v>59</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
@@ -4741,13 +4751,13 @@
         <v>62</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J47" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K47" s="10">
         <v>846921898</v>
@@ -4756,16 +4766,16 @@
         <v>9</v>
       </c>
       <c r="M47" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="N47" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="N47" s="2" t="s">
-        <v>381</v>
-      </c>
       <c r="O47" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4776,10 +4786,10 @@
         <v>60</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="17" t="s">
@@ -4789,13 +4799,13 @@
         <v>61</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J48" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K48" s="14">
         <v>500063557</v>
@@ -4804,25 +4814,28 @@
         <v>2295904</v>
       </c>
       <c r="M48" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="N48" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="N48" s="2" t="s">
+      <c r="O48" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="P48" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="O48" s="2" t="s">
+      <c r="Q48" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q48" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I45" r:id="rId1" xr:uid="{A6BDBEA4-D6A7-AF4B-ABF0-2F48855A524B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>